<commit_message>
random sample test added
</commit_message>
<xml_diff>
--- a/mkt1ClassifiersResults.xlsx
+++ b/mkt1ClassifiersResults.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="77">
   <si>
     <t>Var. gp</t>
   </si>
@@ -180,9 +180,6 @@
     <t>Features used</t>
   </si>
   <si>
-    <t>penalty l1, c=0.1</t>
-  </si>
-  <si>
     <t>Y add. Ratio sign</t>
   </si>
   <si>
@@ -205,9 +202,6 @@
   </si>
   <si>
     <t>Y rest sum func p stck magnitude</t>
-  </si>
-  <si>
-    <t>penalty l2, c=0.1</t>
   </si>
   <si>
     <t>Notes:</t>
@@ -233,12 +227,33 @@
   <si>
     <t>The logistic regression does not use the stocks for the prediction, as difference in stock number is not relevant. Implementing a proper metric caused performance issues so far.</t>
   </si>
+  <si>
+    <t>l1</t>
+  </si>
+  <si>
+    <t>l2</t>
+  </si>
+  <si>
+    <t>Repeated K-folds</t>
+  </si>
+  <si>
+    <t>Random samples</t>
+  </si>
+  <si>
+    <t>Changing the testing methodology from K-fold to random changes completely the scores, and make logistic regression model usable in a few cases</t>
+  </si>
+  <si>
+    <t>Penalty</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,8 +286,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,6 +307,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,7 +571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -562,16 +593,46 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5625,1508 +5686,3415 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H74"/>
+  <dimension ref="A1:L136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L1" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L2" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L3" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L4" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L6" s="24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L7" s="24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L8" s="24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L9" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L10" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F15" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="27"/>
+      <c r="H15" s="25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B16" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F16" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G16" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="H16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="34">
+        <v>0.1</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="29">
+        <v>4.04</v>
+      </c>
+      <c r="G17" s="29">
+        <v>4.0179999999999998</v>
+      </c>
+      <c r="H17" s="10">
+        <v>8.0779999999999994</v>
+      </c>
+      <c r="I17" s="10">
+        <v>8.0670000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="30">
+        <v>4.0279999999999996</v>
+      </c>
+      <c r="G18" s="30">
+        <v>4.0129999999999999</v>
+      </c>
+      <c r="H18" s="5">
+        <v>8.0540000000000003</v>
+      </c>
+      <c r="I18" s="5">
+        <v>8.0389999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="30">
+        <v>4.0309999999999997</v>
+      </c>
+      <c r="G19" s="30">
+        <v>4.0259999999999998</v>
+      </c>
+      <c r="H19" s="5">
+        <v>8.0579999999999998</v>
+      </c>
+      <c r="I19" s="5">
+        <v>8.0630000000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="30">
+        <v>4.16</v>
+      </c>
+      <c r="G20" s="30">
+        <v>4.125</v>
+      </c>
+      <c r="H20" s="5">
+        <v>8.3089999999999993</v>
+      </c>
+      <c r="I20" s="5">
+        <v>8.2729999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="30">
+        <v>4.016</v>
+      </c>
+      <c r="G21" s="30">
+        <v>4.0140000000000002</v>
+      </c>
+      <c r="H21" s="5">
+        <v>8.0269999999999992</v>
+      </c>
+      <c r="I21" s="5">
+        <v>8.0419999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="30">
+        <v>4.0149999999999997</v>
+      </c>
+      <c r="G22" s="30">
+        <v>4.0129999999999999</v>
+      </c>
+      <c r="H22" s="5">
+        <v>8.0269999999999992</v>
+      </c>
+      <c r="I22" s="5">
+        <v>8.0359999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="30">
+        <v>36.82</v>
+      </c>
+      <c r="G23" s="30">
+        <v>36.817</v>
+      </c>
+      <c r="H23" s="5">
+        <v>73.626999999999995</v>
+      </c>
+      <c r="I23" s="5">
+        <v>73.67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="30">
+        <v>36.832999999999998</v>
+      </c>
+      <c r="G24" s="30">
+        <v>36.825000000000003</v>
+      </c>
+      <c r="H24" s="5">
+        <v>73.652000000000001</v>
+      </c>
+      <c r="I24" s="5">
+        <v>73.691999999999993</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" s="30">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="G25" s="30">
+        <v>36.838999999999999</v>
+      </c>
+      <c r="H25" s="5">
+        <v>73.668000000000006</v>
+      </c>
+      <c r="I25" s="5">
+        <v>73.716999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="30">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="G26" s="30">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="H26" s="5">
+        <v>73.668000000000006</v>
+      </c>
+      <c r="I26" s="5">
+        <v>73.716999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="30">
+        <v>36.841000000000001</v>
+      </c>
+      <c r="G27" s="30">
+        <v>36.838999999999999</v>
+      </c>
+      <c r="H27" s="5">
+        <v>73.67</v>
+      </c>
+      <c r="I27" s="5">
+        <v>73.715000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="30">
+        <v>36.841000000000001</v>
+      </c>
+      <c r="G28" s="30">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="H28" s="5">
+        <v>73.668999999999997</v>
+      </c>
+      <c r="I28" s="5">
+        <v>73.715999999999994</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="E29" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="5">
+        <v>73.679000000000002</v>
+      </c>
+      <c r="I29" s="5">
+        <v>73.710999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="5">
+        <v>73.765000000000001</v>
+      </c>
+      <c r="I30" s="5">
+        <v>73.787999999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="5">
+        <v>73.665999999999997</v>
+      </c>
+      <c r="I31" s="5">
+        <v>73.715000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="5">
+        <v>73.679000000000002</v>
+      </c>
+      <c r="I32" s="5">
+        <v>73.724000000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="5">
+        <v>73.665999999999997</v>
+      </c>
+      <c r="I33" s="5">
+        <v>73.710999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="5">
+        <v>73.668000000000006</v>
+      </c>
+      <c r="I34" s="5">
+        <v>73.715999999999994</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="5">
+        <v>86.918999999999997</v>
+      </c>
+      <c r="I35" s="5">
+        <v>86.88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="5">
+        <v>86.941999999999993</v>
+      </c>
+      <c r="I36" s="5">
+        <v>86.888000000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="5">
+        <v>86.929000000000002</v>
+      </c>
+      <c r="I37" s="5">
+        <v>86.908000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="5">
+        <v>86.924999999999997</v>
+      </c>
+      <c r="I38" s="5">
+        <v>86.897999999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="5">
+        <v>86.924000000000007</v>
+      </c>
+      <c r="I39" s="5">
+        <v>86.902000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="5">
+        <v>86.929000000000002</v>
+      </c>
+      <c r="I40" s="5">
+        <v>86.906999999999996</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="5">
+        <v>54.673000000000002</v>
+      </c>
+      <c r="I41" s="5">
+        <v>54.603000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="5">
+        <v>54.720999999999997</v>
+      </c>
+      <c r="I42" s="5">
+        <v>54.646000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" s="30"/>
+      <c r="G43" s="30"/>
+      <c r="H43" s="5">
+        <v>54.725999999999999</v>
+      </c>
+      <c r="I43" s="5">
+        <v>54.664000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F44" s="30"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="5">
+        <v>54.673000000000002</v>
+      </c>
+      <c r="I44" s="5">
+        <v>54.598999999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F45" s="30"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="5">
+        <v>54.725999999999999</v>
+      </c>
+      <c r="I45" s="5">
+        <v>54.661000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F46" s="30"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="5">
+        <v>54.728000000000002</v>
+      </c>
+      <c r="I46" s="5">
+        <v>54.664999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F47" s="30"/>
+      <c r="G47" s="30"/>
+      <c r="H47" s="5">
+        <v>52.68</v>
+      </c>
+      <c r="I47" s="5">
+        <v>52.564999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="5">
+        <v>52.540999999999997</v>
+      </c>
+      <c r="I48" s="5">
+        <v>52.491999999999997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F49" s="30"/>
+      <c r="G49" s="30"/>
+      <c r="H49" s="5">
+        <v>52.064</v>
+      </c>
+      <c r="I49" s="5">
+        <v>51.999000000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B50" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F50" s="30"/>
+      <c r="G50" s="30"/>
+      <c r="H50" s="5">
+        <v>55.545000000000002</v>
+      </c>
+      <c r="I50" s="5">
+        <v>55.503</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F51" s="30"/>
+      <c r="G51" s="30"/>
+      <c r="H51" s="5">
+        <v>51.981999999999999</v>
+      </c>
+      <c r="I51" s="5">
+        <v>51.905000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F52" s="30"/>
+      <c r="G52" s="30"/>
+      <c r="H52" s="5">
+        <v>51.994</v>
+      </c>
+      <c r="I52" s="5">
+        <v>51.920999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F53" s="30"/>
+      <c r="G53" s="30"/>
+      <c r="H53" s="5">
+        <v>54.991999999999997</v>
+      </c>
+      <c r="I53" s="5">
+        <v>54.887</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C54" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F54" s="30"/>
+      <c r="G54" s="30"/>
+      <c r="H54" s="5">
+        <v>54.753999999999998</v>
+      </c>
+      <c r="I54" s="5">
+        <v>54.658000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B55" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F55" s="30"/>
+      <c r="G55" s="30"/>
+      <c r="H55" s="5">
+        <v>54.722999999999999</v>
+      </c>
+      <c r="I55" s="5">
+        <v>54.66</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B56" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F56" s="30"/>
+      <c r="G56" s="30"/>
+      <c r="H56" s="5">
+        <v>54.965000000000003</v>
+      </c>
+      <c r="I56" s="5">
+        <v>54.893000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B57" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F57" s="30"/>
+      <c r="G57" s="30"/>
+      <c r="H57" s="5">
+        <v>54.713000000000001</v>
+      </c>
+      <c r="I57" s="5">
+        <v>54.628</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B58" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F58" s="30"/>
+      <c r="G58" s="30"/>
+      <c r="H58" s="5">
+        <v>54.726999999999997</v>
+      </c>
+      <c r="I58" s="5">
+        <v>54.661000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F59" s="30"/>
+      <c r="G59" s="30"/>
+      <c r="H59" s="5">
+        <v>30.701000000000001</v>
+      </c>
+      <c r="I59" s="5">
+        <v>30.754999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B60" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F60" s="30"/>
+      <c r="G60" s="30"/>
+      <c r="H60" s="5">
+        <v>30.071000000000002</v>
+      </c>
+      <c r="I60" s="5">
+        <v>30.106000000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F61" s="30"/>
+      <c r="G61" s="30"/>
+      <c r="H61" s="5">
+        <v>30.35</v>
+      </c>
+      <c r="I61" s="5">
+        <v>30.425999999999998</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B62" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F62" s="30"/>
+      <c r="G62" s="30"/>
+      <c r="H62" s="5">
+        <v>30.734999999999999</v>
+      </c>
+      <c r="I62" s="5">
+        <v>30.782</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B63" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F63" s="30"/>
+      <c r="G63" s="30"/>
+      <c r="H63" s="5">
+        <v>29.981999999999999</v>
+      </c>
+      <c r="I63" s="5">
+        <v>30.042000000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B64" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F64" s="30"/>
+      <c r="G64" s="30"/>
+      <c r="H64" s="5">
+        <v>29.989000000000001</v>
+      </c>
+      <c r="I64" s="5">
+        <v>30.044</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B65" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C65" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F65" s="30"/>
+      <c r="G65" s="30"/>
+      <c r="H65" s="5">
+        <v>59.335999999999999</v>
+      </c>
+      <c r="I65" s="5">
+        <v>59.338000000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B66" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F66" s="30"/>
+      <c r="G66" s="30"/>
+      <c r="H66" s="5">
+        <v>60.017000000000003</v>
+      </c>
+      <c r="I66" s="5">
+        <v>60.003</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B67" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C67" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F67" s="30"/>
+      <c r="G67" s="30"/>
+      <c r="H67" s="5">
+        <v>59.296999999999997</v>
+      </c>
+      <c r="I67" s="5">
+        <v>59.314</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B68" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C68" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F68" s="30"/>
+      <c r="G68" s="30"/>
+      <c r="H68" s="5">
+        <v>59.728999999999999</v>
+      </c>
+      <c r="I68" s="5">
+        <v>59.68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B69" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C69" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F69" s="30"/>
+      <c r="G69" s="30"/>
+      <c r="H69" s="5">
+        <v>59.412999999999997</v>
+      </c>
+      <c r="I69" s="5">
+        <v>59.423999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B70" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C70" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F70" s="30"/>
+      <c r="G70" s="30"/>
+      <c r="H70" s="5">
+        <v>59.41</v>
+      </c>
+      <c r="I70" s="5">
+        <v>59.421999999999997</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B71" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C71" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F71" s="30"/>
+      <c r="G71" s="30"/>
+      <c r="H71" s="5">
+        <v>40.298999999999999</v>
+      </c>
+      <c r="I71" s="5">
+        <v>40.386000000000003</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B72" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C72" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F72" s="30"/>
+      <c r="G72" s="30"/>
+      <c r="H72" s="5">
+        <v>40.277000000000001</v>
+      </c>
+      <c r="I72" s="5">
+        <v>40.363999999999997</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B73" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C73" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F73" s="30"/>
+      <c r="G73" s="30"/>
+      <c r="H73" s="5">
+        <v>40.250999999999998</v>
+      </c>
+      <c r="I73" s="5">
+        <v>40.36</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B74" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C74" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F74" s="30"/>
+      <c r="G74" s="30"/>
+      <c r="H74" s="5">
+        <v>40.243000000000002</v>
+      </c>
+      <c r="I74" s="5">
+        <v>40.343000000000004</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B75" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C75" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F75" s="30"/>
+      <c r="G75" s="30"/>
+      <c r="H75" s="5">
+        <v>40.273000000000003</v>
+      </c>
+      <c r="I75" s="5">
+        <v>40.375999999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B76" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C76" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="D76" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E76" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F76" s="31"/>
+      <c r="G76" s="31"/>
+      <c r="H76" s="20">
+        <v>40.274000000000001</v>
+      </c>
+      <c r="I76" s="20">
+        <v>40.372999999999998</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B77" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C77" s="39">
+        <v>0.1</v>
+      </c>
+      <c r="D77" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E77" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="10">
-        <v>4.04</v>
-      </c>
-      <c r="F3" s="10">
-        <v>4.0179999999999998</v>
-      </c>
-      <c r="H3" s="28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="F77" s="32">
+        <v>4.0419999999999998</v>
+      </c>
+      <c r="G77" s="32">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="H77" s="22">
+        <v>8.0850000000000009</v>
+      </c>
+      <c r="I77" s="22">
+        <v>8.0609999999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B78" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C78" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F78" s="30">
+        <v>4.0270000000000001</v>
+      </c>
+      <c r="G78" s="30">
+        <v>4.0110000000000001</v>
+      </c>
+      <c r="H78" s="5">
+        <v>8.0570000000000004</v>
+      </c>
+      <c r="I78" s="5">
+        <v>8.0370000000000008</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B79" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C79" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F79" s="30">
+        <v>4.0270000000000001</v>
+      </c>
+      <c r="G79" s="30">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="H79" s="5">
+        <v>8.0519999999999996</v>
+      </c>
+      <c r="I79" s="5">
+        <v>8.0540000000000003</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B80" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C80" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F80" s="30">
+        <v>4.1689999999999996</v>
+      </c>
+      <c r="G80" s="30">
+        <v>4.1440000000000001</v>
+      </c>
+      <c r="H80" s="5">
+        <v>8.3390000000000004</v>
+      </c>
+      <c r="I80" s="5">
+        <v>8.298</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B81" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C81" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F81" s="30">
+        <v>4.0170000000000003</v>
+      </c>
+      <c r="G81" s="30">
+        <v>4.0140000000000002</v>
+      </c>
+      <c r="H81" s="5">
+        <v>8.0269999999999992</v>
+      </c>
+      <c r="I81" s="5">
+        <v>8.0429999999999993</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B82" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C82" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F82" s="30">
+        <v>2.96</v>
+      </c>
+      <c r="G82" s="30">
+        <v>2.9940000000000002</v>
+      </c>
+      <c r="H82" s="5">
+        <v>5.0919999999999996</v>
+      </c>
+      <c r="I82" s="5">
+        <v>5.0979999999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B83" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C83" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F83" s="30">
+        <v>36.82</v>
+      </c>
+      <c r="G83" s="30">
+        <v>36.817</v>
+      </c>
+      <c r="H83" s="5">
+        <v>73.626999999999995</v>
+      </c>
+      <c r="I83" s="5">
+        <v>73.668000000000006</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B84" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C84" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F84" s="30">
+        <v>36.832000000000001</v>
+      </c>
+      <c r="G84" s="30">
+        <v>36.825000000000003</v>
+      </c>
+      <c r="H84" s="5">
+        <v>73.650999999999996</v>
+      </c>
+      <c r="I84" s="5">
+        <v>73.691000000000003</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B85" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C85" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F85" s="30">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="G85" s="30">
+        <v>36.838999999999999</v>
+      </c>
+      <c r="H85" s="5">
+        <v>73.667000000000002</v>
+      </c>
+      <c r="I85" s="5">
+        <v>73.716999999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B86" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C86" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F86" s="30">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="G86" s="30">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="H86" s="5">
+        <v>73.668000000000006</v>
+      </c>
+      <c r="I86" s="5">
+        <v>73.716999999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B87" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C87" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F87" s="30">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="G87" s="30">
+        <v>36.837000000000003</v>
+      </c>
+      <c r="H87" s="5">
+        <v>73.668999999999997</v>
+      </c>
+      <c r="I87" s="5">
+        <v>73.713999999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B88" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C88" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F88" s="30">
+        <v>13.117000000000001</v>
+      </c>
+      <c r="G88" s="30">
+        <v>13.081</v>
+      </c>
+      <c r="H88" s="5">
+        <v>36.777999999999999</v>
+      </c>
+      <c r="I88" s="5">
+        <v>36.871000000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B89" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C89" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D89" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="E89" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F89" s="30">
+        <v>36.844999999999999</v>
+      </c>
+      <c r="G89" s="30">
+        <v>36.838999999999999</v>
+      </c>
+      <c r="H89" s="5">
+        <v>73.680000000000007</v>
+      </c>
+      <c r="I89" s="5">
+        <v>73.710999999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B90" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C90" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E90" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="5">
-        <v>4.0279999999999996</v>
-      </c>
-      <c r="F4" s="5">
-        <v>4.0129999999999999</v>
-      </c>
-      <c r="H4" s="28" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="F90" s="30">
+        <v>36.884999999999998</v>
+      </c>
+      <c r="G90" s="30">
+        <v>36.883000000000003</v>
+      </c>
+      <c r="H90" s="5">
+        <v>73.766000000000005</v>
+      </c>
+      <c r="I90" s="5">
+        <v>73.789000000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B91" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C91" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D91" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="E91" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="5">
-        <v>4.0309999999999997</v>
-      </c>
-      <c r="F5" s="5">
-        <v>4.0259999999999998</v>
-      </c>
-      <c r="H5" s="28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="F91" s="30">
+        <v>36.838000000000001</v>
+      </c>
+      <c r="G91" s="30">
+        <v>36.837000000000003</v>
+      </c>
+      <c r="H91" s="5">
+        <v>73.664000000000001</v>
+      </c>
+      <c r="I91" s="5">
+        <v>73.712999999999994</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B92" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C92" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D92" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="E92" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="5">
-        <v>4.16</v>
-      </c>
-      <c r="F6" s="5">
-        <v>4.125</v>
-      </c>
-      <c r="H6" s="28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="6" t="s">
+      <c r="F92" s="30">
+        <v>36.845999999999997</v>
+      </c>
+      <c r="G92" s="30">
+        <v>36.847999999999999</v>
+      </c>
+      <c r="H92" s="5">
+        <v>73.679000000000002</v>
+      </c>
+      <c r="I92" s="5">
+        <v>73.724999999999994</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B93" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C93" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D93" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="E93" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="5">
-        <v>4.016</v>
-      </c>
-      <c r="F7" s="5">
-        <v>4.0140000000000002</v>
-      </c>
-      <c r="H7" s="28" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="6" t="s">
+      <c r="F93" s="30">
+        <v>36.837000000000003</v>
+      </c>
+      <c r="G93" s="30">
+        <v>36.832000000000001</v>
+      </c>
+      <c r="H93" s="5">
+        <v>73.662999999999997</v>
+      </c>
+      <c r="I93" s="5">
+        <v>73.709999999999994</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B94" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C94" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D94" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="E94" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="5">
-        <v>4.0149999999999997</v>
-      </c>
-      <c r="F8" s="5">
-        <v>4.0129999999999999</v>
-      </c>
-      <c r="H8" s="28" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="F94" s="30">
+        <v>15.337999999999999</v>
+      </c>
+      <c r="G94" s="30">
+        <v>15.323</v>
+      </c>
+      <c r="H94" s="5">
+        <v>40.073</v>
+      </c>
+      <c r="I94" s="5">
+        <v>40.131</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B95" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C95" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E95" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="5">
-        <v>36.82</v>
-      </c>
-      <c r="F9" s="5">
-        <v>36.817</v>
-      </c>
-      <c r="H9" s="28" t="s">
+      <c r="F95" s="30">
+        <v>43.454000000000001</v>
+      </c>
+      <c r="G95" s="30">
+        <v>43.448</v>
+      </c>
+      <c r="H95" s="5">
+        <v>86.915000000000006</v>
+      </c>
+      <c r="I95" s="5">
+        <v>86.872</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B96" s="36" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="C96" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E96" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="5">
-        <v>36.832999999999998</v>
-      </c>
-      <c r="F10" s="5">
-        <v>36.825000000000003</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="F96" s="30">
+        <v>43.463999999999999</v>
+      </c>
+      <c r="G96" s="30">
+        <v>43.460999999999999</v>
+      </c>
+      <c r="H96" s="5">
+        <v>86.941000000000003</v>
+      </c>
+      <c r="I96" s="5">
+        <v>86.884</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B97" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C97" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E97" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="5">
-        <v>36.840000000000003</v>
-      </c>
-      <c r="F11" s="5">
-        <v>36.838999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="F97" s="30">
+        <v>43.462000000000003</v>
+      </c>
+      <c r="G97" s="30">
+        <v>43.460999999999999</v>
+      </c>
+      <c r="H97" s="5">
+        <v>86.929000000000002</v>
+      </c>
+      <c r="I97" s="5">
+        <v>86.908000000000001</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B98" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C98" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E98" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="5">
-        <v>36.840000000000003</v>
-      </c>
-      <c r="F12" s="5">
-        <v>36.840000000000003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="F98" s="30">
+        <v>43.462000000000003</v>
+      </c>
+      <c r="G98" s="30">
+        <v>43.46</v>
+      </c>
+      <c r="H98" s="5">
+        <v>86.93</v>
+      </c>
+      <c r="I98" s="5">
+        <v>86.903999999999996</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B99" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C99" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E99" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="5">
-        <v>36.841000000000001</v>
-      </c>
-      <c r="F13" s="5">
-        <v>36.838999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="21" t="s">
+      <c r="F99" s="30">
+        <v>43.46</v>
+      </c>
+      <c r="G99" s="30">
+        <v>43.46</v>
+      </c>
+      <c r="H99" s="5">
+        <v>86.926000000000002</v>
+      </c>
+      <c r="I99" s="5">
+        <v>86.903999999999996</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B100" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C100" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E100" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="22">
-        <v>36.841000000000001</v>
-      </c>
-      <c r="F14" s="22">
-        <v>36.840000000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="25" t="s">
+      <c r="F100" s="30">
+        <v>29.122</v>
+      </c>
+      <c r="G100" s="30">
+        <v>29.122</v>
+      </c>
+      <c r="H100" s="5">
+        <v>58.982999999999997</v>
+      </c>
+      <c r="I100" s="5">
+        <v>58.941000000000003</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B101" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C101" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E101" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="26">
-        <v>4.0419999999999998</v>
-      </c>
-      <c r="F15" s="26">
-        <v>4.0199999999999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="F101" s="30">
+        <v>27.33</v>
+      </c>
+      <c r="G101" s="30">
+        <v>27.323</v>
+      </c>
+      <c r="H101" s="5">
+        <v>54.677</v>
+      </c>
+      <c r="I101" s="5">
+        <v>54.607999999999997</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B102" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C102" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E102" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="5">
-        <v>4.0270000000000001</v>
-      </c>
-      <c r="F16" s="5">
-        <v>4.0110000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="F102" s="30">
+        <v>27.352</v>
+      </c>
+      <c r="G102" s="30">
+        <v>27.347000000000001</v>
+      </c>
+      <c r="H102" s="5">
+        <v>54.72</v>
+      </c>
+      <c r="I102" s="5">
+        <v>54.643000000000001</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B103" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C103" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E103" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="5">
-        <v>4.0270000000000001</v>
-      </c>
-      <c r="F17" s="5">
-        <v>4.0199999999999996</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="F103" s="30">
+        <v>27.355</v>
+      </c>
+      <c r="G103" s="30">
+        <v>27.355</v>
+      </c>
+      <c r="H103" s="5">
+        <v>54.725999999999999</v>
+      </c>
+      <c r="I103" s="5">
+        <v>54.664000000000001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B104" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C104" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E104" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="5">
-        <v>4.1689999999999996</v>
-      </c>
-      <c r="F18" s="5">
-        <v>4.1440000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="F104" s="30">
+        <v>27.326000000000001</v>
+      </c>
+      <c r="G104" s="30">
+        <v>27.323</v>
+      </c>
+      <c r="H104" s="5">
+        <v>54.67</v>
+      </c>
+      <c r="I104" s="5">
+        <v>54.597000000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B105" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C105" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E105" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="5">
-        <v>4.0170000000000003</v>
-      </c>
-      <c r="F19" s="5">
-        <v>4.0140000000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="F105" s="30">
+        <v>27.355</v>
+      </c>
+      <c r="G105" s="30">
+        <v>27.355</v>
+      </c>
+      <c r="H105" s="5">
+        <v>54.725999999999999</v>
+      </c>
+      <c r="I105" s="5">
+        <v>54.661000000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B106" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C106" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E106" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="5">
-        <v>2.96</v>
-      </c>
-      <c r="F20" s="5">
-        <v>2.9940000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="4" t="s">
+      <c r="F106" s="30">
+        <v>14.109</v>
+      </c>
+      <c r="G106" s="30">
+        <v>14.172000000000001</v>
+      </c>
+      <c r="H106" s="5">
+        <v>29.352</v>
+      </c>
+      <c r="I106" s="5">
+        <v>29.462</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B107" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C107" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E107" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="5">
-        <v>36.82</v>
-      </c>
-      <c r="F21" s="5">
-        <v>36.817</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="4" t="s">
+      <c r="F107" s="30">
+        <v>26.376999999999999</v>
+      </c>
+      <c r="G107" s="30">
+        <v>26.37</v>
+      </c>
+      <c r="H107" s="5">
+        <v>52.707000000000001</v>
+      </c>
+      <c r="I107" s="5">
+        <v>52.624000000000002</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B108" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C108" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E108" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="5">
-        <v>36.832000000000001</v>
-      </c>
-      <c r="F22" s="5">
-        <v>36.825000000000003</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="4" t="s">
+      <c r="F108" s="30">
+        <v>26.263999999999999</v>
+      </c>
+      <c r="G108" s="30">
+        <v>26.236999999999998</v>
+      </c>
+      <c r="H108" s="5">
+        <v>52.557000000000002</v>
+      </c>
+      <c r="I108" s="5">
+        <v>52.484000000000002</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B109" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C109" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E109" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="5">
-        <v>36.840000000000003</v>
-      </c>
-      <c r="F23" s="5">
-        <v>36.838999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="4" t="s">
+      <c r="F109" s="30">
+        <v>25.866</v>
+      </c>
+      <c r="G109" s="30">
+        <v>25.853000000000002</v>
+      </c>
+      <c r="H109" s="5">
+        <v>51.725999999999999</v>
+      </c>
+      <c r="I109" s="5">
+        <v>51.77</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B110" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C110" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E110" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E24" s="5">
-        <v>36.840000000000003</v>
-      </c>
-      <c r="F24" s="5">
-        <v>36.840000000000003</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" s="4" t="s">
+      <c r="F110" s="30">
+        <v>27.777999999999999</v>
+      </c>
+      <c r="G110" s="30">
+        <v>27.739000000000001</v>
+      </c>
+      <c r="H110" s="5">
+        <v>55.552</v>
+      </c>
+      <c r="I110" s="5">
+        <v>55.533000000000001</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B111" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C111" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E111" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="5">
-        <v>36.840000000000003</v>
-      </c>
-      <c r="F25" s="5">
-        <v>36.837000000000003</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" s="4" t="s">
+      <c r="F111" s="30">
+        <v>25.888999999999999</v>
+      </c>
+      <c r="G111" s="30">
+        <v>25.832999999999998</v>
+      </c>
+      <c r="H111" s="5">
+        <v>51.798000000000002</v>
+      </c>
+      <c r="I111" s="5">
+        <v>51.802999999999997</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B112" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C112" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E112" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="5">
-        <v>13.117000000000001</v>
-      </c>
-      <c r="F26" s="5">
-        <v>13.081</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="4" t="s">
+      <c r="F112" s="30">
+        <v>24.72</v>
+      </c>
+      <c r="G112" s="30">
+        <v>24.72</v>
+      </c>
+      <c r="H112" s="5">
+        <v>49.465000000000003</v>
+      </c>
+      <c r="I112" s="5">
+        <v>49.588000000000001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B113" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C113" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E113" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="5">
-        <v>36.844999999999999</v>
-      </c>
-      <c r="F27" s="5">
-        <v>36.838999999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28" s="4" t="s">
+      <c r="F113" s="30">
+        <v>27.492000000000001</v>
+      </c>
+      <c r="G113" s="30">
+        <v>27.495999999999999</v>
+      </c>
+      <c r="H113" s="5">
+        <v>55.01</v>
+      </c>
+      <c r="I113" s="5">
+        <v>54.9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B114" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C114" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E114" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="5">
-        <v>36.884999999999998</v>
-      </c>
-      <c r="F28" s="5">
-        <v>36.883000000000003</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="4" t="s">
+      <c r="F114" s="30">
+        <v>27.367000000000001</v>
+      </c>
+      <c r="G114" s="30">
+        <v>27.359000000000002</v>
+      </c>
+      <c r="H114" s="5">
+        <v>54.758000000000003</v>
+      </c>
+      <c r="I114" s="5">
+        <v>54.661000000000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B115" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C115" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D115" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E115" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="5">
-        <v>36.838000000000001</v>
-      </c>
-      <c r="F29" s="5">
-        <v>36.837000000000003</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="4" t="s">
+      <c r="F115" s="30">
+        <v>27.353999999999999</v>
+      </c>
+      <c r="G115" s="30">
+        <v>27.356000000000002</v>
+      </c>
+      <c r="H115" s="5">
+        <v>54.725000000000001</v>
+      </c>
+      <c r="I115" s="5">
+        <v>54.662999999999997</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B116" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C116" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E116" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="5">
-        <v>36.845999999999997</v>
-      </c>
-      <c r="F30" s="5">
-        <v>36.847999999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" s="4" t="s">
+      <c r="F116" s="30">
+        <v>27.475000000000001</v>
+      </c>
+      <c r="G116" s="30">
+        <v>27.48</v>
+      </c>
+      <c r="H116" s="5">
+        <v>54.963000000000001</v>
+      </c>
+      <c r="I116" s="5">
+        <v>54.902999999999999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B117" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C117" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E117" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E31" s="5">
-        <v>36.837000000000003</v>
-      </c>
-      <c r="F31" s="5">
-        <v>36.832000000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="4" t="s">
+      <c r="F117" s="30">
+        <v>27.346</v>
+      </c>
+      <c r="G117" s="30">
+        <v>27.344999999999999</v>
+      </c>
+      <c r="H117" s="5">
+        <v>54.713000000000001</v>
+      </c>
+      <c r="I117" s="5">
+        <v>54.631999999999998</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B118" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C118" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E118" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E32" s="5">
-        <v>15.337999999999999</v>
-      </c>
-      <c r="F32" s="5">
-        <v>15.323</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D33" s="4" t="s">
+      <c r="F118" s="30">
+        <v>21.789000000000001</v>
+      </c>
+      <c r="G118" s="30">
+        <v>21.724</v>
+      </c>
+      <c r="H118" s="5">
+        <v>40.844000000000001</v>
+      </c>
+      <c r="I118" s="5">
+        <v>40.936</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B119" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C119" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D119" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E119" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E33" s="5">
-        <v>43.454000000000001</v>
-      </c>
-      <c r="F33" s="5">
-        <v>43.448</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34" s="4" t="s">
+      <c r="F119" s="30">
+        <v>15.367000000000001</v>
+      </c>
+      <c r="G119" s="30">
+        <v>15.266</v>
+      </c>
+      <c r="H119" s="5">
+        <v>30.704999999999998</v>
+      </c>
+      <c r="I119" s="5">
+        <v>30.753</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B120" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C120" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E120" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E34" s="5">
-        <v>43.463999999999999</v>
-      </c>
-      <c r="F34" s="5">
-        <v>43.460999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D35" s="4" t="s">
+      <c r="F120" s="30">
+        <v>15.041</v>
+      </c>
+      <c r="G120" s="30">
+        <v>15.028</v>
+      </c>
+      <c r="H120" s="5">
+        <v>30.082000000000001</v>
+      </c>
+      <c r="I120" s="5">
+        <v>30.11</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B121" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C121" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D121" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E121" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="5">
-        <v>43.462000000000003</v>
-      </c>
-      <c r="F35" s="5">
-        <v>43.460999999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D36" s="4" t="s">
+      <c r="F121" s="30">
+        <v>15.132</v>
+      </c>
+      <c r="G121" s="30">
+        <v>15.076000000000001</v>
+      </c>
+      <c r="H121" s="5">
+        <v>30.195</v>
+      </c>
+      <c r="I121" s="5">
+        <v>30.277999999999999</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B122" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C122" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E122" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E36" s="5">
-        <v>43.462000000000003</v>
-      </c>
-      <c r="F36" s="5">
-        <v>43.46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D37" s="4" t="s">
+      <c r="F122" s="30">
+        <v>15.391</v>
+      </c>
+      <c r="G122" s="30">
+        <v>15.27</v>
+      </c>
+      <c r="H122" s="5">
+        <v>30.704999999999998</v>
+      </c>
+      <c r="I122" s="5">
+        <v>30.765999999999998</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B123" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C123" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E123" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E37" s="5">
-        <v>43.46</v>
-      </c>
-      <c r="F37" s="5">
-        <v>43.46</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D38" s="4" t="s">
+      <c r="F123" s="30">
+        <v>15.000999999999999</v>
+      </c>
+      <c r="G123" s="30">
+        <v>14.977</v>
+      </c>
+      <c r="H123" s="5">
+        <v>29.981999999999999</v>
+      </c>
+      <c r="I123" s="5">
+        <v>30.038</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B124" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C124" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E124" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E38" s="5">
-        <v>29.122</v>
-      </c>
-      <c r="F38" s="5">
-        <v>29.122</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" s="4" t="s">
+      <c r="F124" s="30">
+        <v>10.923</v>
+      </c>
+      <c r="G124" s="30">
+        <v>10.984999999999999</v>
+      </c>
+      <c r="H124" s="5">
+        <v>22.606999999999999</v>
+      </c>
+      <c r="I124" s="5">
+        <v>22.632000000000001</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B125" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C125" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E125" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="5">
-        <v>27.33</v>
-      </c>
-      <c r="F39" s="5">
-        <v>27.323</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D40" s="4" t="s">
+      <c r="F125" s="30">
+        <v>29.664999999999999</v>
+      </c>
+      <c r="G125" s="30">
+        <v>29.658999999999999</v>
+      </c>
+      <c r="H125" s="5">
+        <v>59.332999999999998</v>
+      </c>
+      <c r="I125" s="5">
+        <v>59.335999999999999</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B126" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C126" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E126" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="5">
-        <v>27.352</v>
-      </c>
-      <c r="F40" s="5">
-        <v>27.347000000000001</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D41" s="4" t="s">
+      <c r="F126" s="30">
+        <v>30.01</v>
+      </c>
+      <c r="G126" s="30">
+        <v>30</v>
+      </c>
+      <c r="H126" s="5">
+        <v>60.021999999999998</v>
+      </c>
+      <c r="I126" s="5">
+        <v>60.017000000000003</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B127" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C127" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D127" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E127" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E41" s="5">
-        <v>27.355</v>
-      </c>
-      <c r="F41" s="5">
-        <v>27.355</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D42" s="4" t="s">
+      <c r="F127" s="30">
+        <v>29.696999999999999</v>
+      </c>
+      <c r="G127" s="30">
+        <v>29.69</v>
+      </c>
+      <c r="H127" s="5">
+        <v>59.365000000000002</v>
+      </c>
+      <c r="I127" s="5">
+        <v>59.372</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B128" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C128" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D128" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E128" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E42" s="5">
-        <v>27.326000000000001</v>
-      </c>
-      <c r="F42" s="5">
-        <v>27.323</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D43" s="4" t="s">
+      <c r="F128" s="30">
+        <v>29.870999999999999</v>
+      </c>
+      <c r="G128" s="30">
+        <v>29.788</v>
+      </c>
+      <c r="H128" s="5">
+        <v>59.725000000000001</v>
+      </c>
+      <c r="I128" s="5">
+        <v>59.682000000000002</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B129" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C129" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E129" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E43" s="5">
-        <v>27.355</v>
-      </c>
-      <c r="F43" s="5">
-        <v>27.355</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D44" s="4" t="s">
+      <c r="F129" s="30">
+        <v>29.707000000000001</v>
+      </c>
+      <c r="G129" s="30">
+        <v>29.704000000000001</v>
+      </c>
+      <c r="H129" s="5">
+        <v>59.412999999999997</v>
+      </c>
+      <c r="I129" s="5">
+        <v>59.423999999999999</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B130" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C130" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E130" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E44" s="5">
-        <v>14.109</v>
-      </c>
-      <c r="F44" s="5">
-        <v>14.172000000000001</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D45" s="4" t="s">
+      <c r="F130" s="30">
+        <v>23.952000000000002</v>
+      </c>
+      <c r="G130" s="30">
+        <v>23.95</v>
+      </c>
+      <c r="H130" s="5">
+        <v>48.332999999999998</v>
+      </c>
+      <c r="I130" s="5">
+        <v>48.29</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B131" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C131" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D131" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E131" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E45" s="5">
-        <v>26.376999999999999</v>
-      </c>
-      <c r="F45" s="5">
-        <v>26.37</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D46" s="4" t="s">
+      <c r="F131" s="30">
+        <v>20.169</v>
+      </c>
+      <c r="G131" s="30">
+        <v>20.094999999999999</v>
+      </c>
+      <c r="H131" s="5">
+        <v>40.296999999999997</v>
+      </c>
+      <c r="I131" s="5">
+        <v>40.384999999999998</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B132" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C132" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D132" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E132" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E46" s="5">
-        <v>26.263999999999999</v>
-      </c>
-      <c r="F46" s="5">
-        <v>26.236999999999998</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D47" s="4" t="s">
+      <c r="F132" s="30">
+        <v>20.152000000000001</v>
+      </c>
+      <c r="G132" s="30">
+        <v>20.141999999999999</v>
+      </c>
+      <c r="H132" s="5">
+        <v>40.277000000000001</v>
+      </c>
+      <c r="I132" s="5">
+        <v>40.363</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B133" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C133" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D133" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E133" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E47" s="5">
-        <v>25.866</v>
-      </c>
-      <c r="F47" s="5">
-        <v>25.853000000000002</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D48" s="4" t="s">
+      <c r="F133" s="30">
+        <v>20.146999999999998</v>
+      </c>
+      <c r="G133" s="30">
+        <v>20.108000000000001</v>
+      </c>
+      <c r="H133" s="5">
+        <v>40.250999999999998</v>
+      </c>
+      <c r="I133" s="5">
+        <v>40.36</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B134" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C134" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D134" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E134" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E48" s="5">
-        <v>27.777999999999999</v>
-      </c>
-      <c r="F48" s="5">
-        <v>27.739000000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D49" s="4" t="s">
+      <c r="F134" s="30">
+        <v>20.143999999999998</v>
+      </c>
+      <c r="G134" s="30">
+        <v>20.097999999999999</v>
+      </c>
+      <c r="H134" s="5">
+        <v>40.241999999999997</v>
+      </c>
+      <c r="I134" s="5">
+        <v>40.344000000000001</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B135" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C135" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E135" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E49" s="5">
-        <v>25.888999999999999</v>
-      </c>
-      <c r="F49" s="5">
-        <v>25.832999999999998</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D50" s="4" t="s">
+      <c r="F135" s="30">
+        <v>20.149999999999999</v>
+      </c>
+      <c r="G135" s="30">
+        <v>20.146000000000001</v>
+      </c>
+      <c r="H135" s="5">
+        <v>40.271999999999998</v>
+      </c>
+      <c r="I135" s="5">
+        <v>40.375999999999998</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B136" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C136" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="D136" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E136" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="E50" s="5">
-        <v>24.72</v>
-      </c>
-      <c r="F50" s="5">
-        <v>24.72</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E51" s="5">
-        <v>27.492000000000001</v>
-      </c>
-      <c r="F51" s="5">
-        <v>27.495999999999999</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E52" s="5">
-        <v>27.367000000000001</v>
-      </c>
-      <c r="F52" s="5">
-        <v>27.359000000000002</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E53" s="5">
-        <v>27.353999999999999</v>
-      </c>
-      <c r="F53" s="5">
-        <v>27.356000000000002</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E54" s="5">
-        <v>27.475000000000001</v>
-      </c>
-      <c r="F54" s="5">
-        <v>27.48</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E55" s="5">
-        <v>27.346</v>
-      </c>
-      <c r="F55" s="5">
-        <v>27.344999999999999</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E56" s="5">
-        <v>21.789000000000001</v>
-      </c>
-      <c r="F56" s="5">
-        <v>21.724</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E57" s="5">
-        <v>15.367000000000001</v>
-      </c>
-      <c r="F57" s="5">
-        <v>15.266</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E58" s="5">
-        <v>15.041</v>
-      </c>
-      <c r="F58" s="5">
-        <v>15.028</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E59" s="5">
-        <v>15.132</v>
-      </c>
-      <c r="F59" s="5">
-        <v>15.076000000000001</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E60" s="5">
-        <v>15.391</v>
-      </c>
-      <c r="F60" s="5">
-        <v>15.27</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E61" s="5">
-        <v>15.000999999999999</v>
-      </c>
-      <c r="F61" s="5">
-        <v>14.977</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E62" s="5">
-        <v>10.923</v>
-      </c>
-      <c r="F62" s="5">
-        <v>10.984999999999999</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E63" s="5">
-        <v>29.664999999999999</v>
-      </c>
-      <c r="F63" s="5">
-        <v>29.658999999999999</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E64" s="5">
-        <v>30.01</v>
-      </c>
-      <c r="F64" s="5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E65" s="5">
-        <v>29.696999999999999</v>
-      </c>
-      <c r="F65" s="5">
-        <v>29.69</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E66" s="5">
-        <v>29.870999999999999</v>
-      </c>
-      <c r="F66" s="5">
-        <v>29.788</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E67" s="5">
-        <v>29.707000000000001</v>
-      </c>
-      <c r="F67" s="5">
-        <v>29.704000000000001</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E68" s="5">
-        <v>23.952000000000002</v>
-      </c>
-      <c r="F68" s="5">
-        <v>23.95</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E69" s="5">
-        <v>20.169</v>
-      </c>
-      <c r="F69" s="5">
-        <v>20.094999999999999</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E70" s="5">
-        <v>20.152000000000001</v>
-      </c>
-      <c r="F70" s="5">
-        <v>20.141999999999999</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E71" s="5">
-        <v>20.146999999999998</v>
-      </c>
-      <c r="F71" s="5">
-        <v>20.108000000000001</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E72" s="5">
-        <v>20.143999999999998</v>
-      </c>
-      <c r="F72" s="5">
-        <v>20.097999999999999</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E73" s="5">
-        <v>20.149999999999999</v>
-      </c>
-      <c r="F73" s="5">
-        <v>20.146000000000001</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B74" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C74" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D74" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E74" s="22">
+      <c r="F136" s="31">
         <v>12.827</v>
       </c>
-      <c r="F74" s="22">
+      <c r="G136" s="31">
         <v>12.891</v>
       </c>
+      <c r="H136" s="20">
+        <v>24.832999999999998</v>
+      </c>
+      <c r="I136" s="20">
+        <v>24.876999999999999</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F17:I136">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -7136,15 +9104,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="H60" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A38" sqref="A1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <sortState ref="A2:H73">
-    <sortCondition ref="C2:C73"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>